<commit_message>
selecting array and delete it
</commit_message>
<xml_diff>
--- a/Untitled spreadsheet.xlsx
+++ b/Untitled spreadsheet.xlsx
@@ -26,14 +26,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -55,14 +51,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -282,34 +275,25 @@
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="B1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1">
-        <v>2.0</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1">
-        <v>3.0</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="B1"/>
-    <hyperlink r:id="rId2" ref="B2"/>
-    <hyperlink r:id="rId3" ref="B3"/>
+    <hyperlink r:id="rId1" ref="A1"/>
+    <hyperlink r:id="rId2" ref="A2"/>
+    <hyperlink r:id="rId3" ref="A3"/>
   </hyperlinks>
   <drawing r:id="rId4"/>
 </worksheet>

</xml_diff>